<commit_message>
may commit for office
</commit_message>
<xml_diff>
--- a/doc/progress_tracker_2021.xlsx
+++ b/doc/progress_tracker_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaker\GoogleDrive\HEBEC\Thesis\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaker\Documents\Thesis\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86827B85-7E92-44CB-9AFE-DD7A91A186A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC715526-8ADE-4A12-BB2D-FEA84A21086F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="9135" windowWidth="19050" windowHeight="6465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29100" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="9" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Wordcount" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="203">
   <si>
     <t>Section</t>
   </si>
@@ -461,9 +462,6 @@
     <t>Progress summary</t>
   </si>
   <si>
-    <t>Next action</t>
-  </si>
-  <si>
     <t>Submission target</t>
   </si>
   <si>
@@ -656,48 +654,9 @@
     <t>Submit to Andrew</t>
   </si>
   <si>
-    <t>Chapter preamble</t>
-  </si>
-  <si>
-    <t>Chapter preamble, peer review</t>
-  </si>
-  <si>
-    <t>Wait for S</t>
-  </si>
-  <si>
-    <t>paste in some formulae and diagrams</t>
-  </si>
-  <si>
     <t>Part</t>
   </si>
   <si>
-    <t>Weeks writing</t>
-  </si>
-  <si>
-    <t>Total weeks</t>
-  </si>
-  <si>
-    <t>TOTAL WEEKS</t>
-  </si>
-  <si>
-    <t>Start estimate</t>
-  </si>
-  <si>
-    <t>Estimated finish</t>
-  </si>
-  <si>
-    <t>First review</t>
-  </si>
-  <si>
-    <t>Second review</t>
-  </si>
-  <si>
-    <t>Send to S</t>
-  </si>
-  <si>
-    <t>Send to A</t>
-  </si>
-  <si>
     <t>Unstructured notes</t>
   </si>
   <si>
@@ -729,6 +688,24 @@
   </si>
   <si>
     <t>Estimate end</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>S comments</t>
+  </si>
+  <si>
+    <t>Revise</t>
+  </si>
+  <si>
+    <t>A comments</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -765,12 +742,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -785,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -794,6 +783,8 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1127,35 +1118,35 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C1" s="4">
         <f ca="1">TODAY()</f>
-        <v>44298</v>
+        <v>44343</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="5">
         <v>44222</v>
       </c>
       <c r="G2">
         <f ca="1">C1-C2</f>
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="H2">
         <f ca="1">0.8*G2</f>
-        <v>60.800000000000004</v>
+        <v>96.800000000000011</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" s="4">
         <f>D14</f>
@@ -1163,12 +1154,12 @@
       </c>
       <c r="D3">
         <f ca="1">C3-C1</f>
-        <v>36</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="4">
         <f>F14</f>
@@ -1187,34 +1178,34 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1222,20 +1213,20 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" ref="D7:D14" si="0">IF(I7&lt;2,$C$2+H7,H7+_xlfn.XLOOKUP(I7-1,I$7:I$14,D$7:D$14,0))</f>
+        <f t="shared" ref="D7:D14" si="0">_xlfn.SINGLE(IF(I7&lt;2,$C$2+H7,H7+_xlfn.XLOOKUP(I7-1,I$7:I$14,D$7:D$14,0)))</f>
         <v>44229</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" ref="F7:F14" si="1">IF(I7&lt;2,$C$3+ROUNDDOWN(1.2*E7,0),ROUNDDOWN(1.2*E7,0)+_xlfn.XLOOKUP(I7-1,I$7:I$14,F$7:F$14,0))</f>
+        <f t="shared" ref="F7:F14" si="1">_xlfn.SINGLE(IF(I7&lt;2,$C$3+ROUNDDOWN(1.2*E7,0),ROUNDDOWN(1.2*E7,0)+_xlfn.XLOOKUP(I7-1,I$7:I$14,F$7:F$14,0)))</f>
         <v>44340</v>
       </c>
       <c r="G7">
@@ -1251,13 +1242,13 @@
       </c>
       <c r="J7" s="6">
         <f t="shared" ref="J7:J14" ca="1" si="4">D7-TODAY()</f>
-        <v>-69</v>
+        <v>-114</v>
       </c>
       <c r="K7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L7" t="s">
         <v>131</v>
-      </c>
-      <c r="L7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1265,7 +1256,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -1293,7 +1284,7 @@
       </c>
       <c r="J8" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>-12</v>
+        <v>-57</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1301,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9">
         <v>15</v>
@@ -1330,7 +1321,7 @@
       </c>
       <c r="J9" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>-36</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1338,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -1367,7 +1358,7 @@
       </c>
       <c r="J10" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>16</v>
+        <v>-29</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1404,7 +1395,7 @@
       </c>
       <c r="J11" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>23</v>
+        <v>-22</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1412,7 +1403,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -1441,13 +1432,13 @@
       </c>
       <c r="J12" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>27</v>
+        <v>-18</v>
       </c>
       <c r="K12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1455,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1484,12 +1475,12 @@
       </c>
       <c r="J13" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>29</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -1518,7 +1509,7 @@
       </c>
       <c r="J14" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>36</v>
+        <v>-9</v>
       </c>
     </row>
   </sheetData>
@@ -1535,18 +1526,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1558,7 +1549,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -1567,29 +1558,23 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>197</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>121</v>
+        <v>198</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>199</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1600,19 +1585,6 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0.5</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <f>SUM(F4:G4)</f>
-        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1621,24 +1593,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>188</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <f>SUM(F5:G5)</f>
-        <v>1</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1648,18 +1607,11 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>188</v>
-      </c>
-      <c r="I6">
-        <f>SUM(F6:G6)</f>
-        <v>0</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -1669,129 +1621,57 @@
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>186</v>
-      </c>
-      <c r="I7">
-        <f>SUM(F7:G7)</f>
-        <v>0</v>
-      </c>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>189</v>
-      </c>
-      <c r="I8">
-        <f>SUM(F8:G8)</f>
-        <v>0</v>
-      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>187</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <f>SUM(F9:G9)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <f>SUM(F10:G10)</f>
-        <v>2</v>
-      </c>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0.5</v>
-      </c>
-      <c r="I11">
-        <f>SUM(F11:G11)</f>
-        <v>0.5</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12">
-        <v>6</v>
-      </c>
-      <c r="H12" t="s">
-        <v>193</v>
-      </c>
-      <c r="I12">
-        <f>SUM(I4:I11)</f>
-        <v>6</v>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>194</v>
-      </c>
-      <c r="I13" s="4">
-        <v>44298</v>
-      </c>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H14" t="s">
-        <v>195</v>
-      </c>
-      <c r="I14" s="4">
-        <f>I13+7*I12</f>
-        <v>44340</v>
-      </c>
+      <c r="I14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -1811,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1819,7 +1699,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1827,7 +1707,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1835,7 +1715,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1843,7 +1723,7 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1862,16 +1742,16 @@
         <v>3</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1879,7 +1759,7 @@
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="E27">
         <v>0.5</v>
@@ -1897,10 +1777,10 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D28" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="F28">
         <v>0.5</v>
@@ -1915,10 +1795,10 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D29" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="F29">
         <v>0.5</v>
@@ -1936,7 +1816,7 @@
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="F30">
         <v>0.2</v>
@@ -1951,7 +1831,7 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E31">
         <v>0.5</v>
@@ -1972,7 +1852,7 @@
         <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="F32">
         <v>0.2</v>
@@ -1990,7 +1870,7 @@
         <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -2011,7 +1891,7 @@
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="E34">
         <v>0.5</v>
@@ -2029,7 +1909,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="H35">
         <f>INT(SUM(H27:H34))</f>
@@ -2038,7 +1918,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="H36" s="7">
         <v>44298</v>
@@ -2046,7 +1926,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="H37" s="4">
         <f>H36+H35*7</f>
@@ -2066,8 +1946,8 @@
       <c r="A41" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D4:D13">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="D13">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2130,13 +2010,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
         <v>138</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>139</v>
-      </c>
-      <c r="D2" t="s">
-        <v>140</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2154,13 +2034,13 @@
       </c>
       <c r="B3" s="1"/>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -2169,13 +2049,13 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="D4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -2184,13 +2064,13 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -2201,16 +2081,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
         <v>143</v>
       </c>
-      <c r="C6" t="s">
-        <v>144</v>
-      </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -2218,10 +2098,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" t="s">
         <v>145</v>
-      </c>
-      <c r="D7" t="s">
-        <v>146</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2230,7 +2110,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2239,7 +2119,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="D9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2248,7 +2128,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2258,7 +2138,7 @@
       <c r="A11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2267,10 +2147,10 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2279,7 +2159,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="D13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2288,7 +2168,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="D14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2298,7 +2178,7 @@
       <c r="A15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2308,7 +2188,7 @@
       <c r="A16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2318,7 +2198,7 @@
       <c r="A17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -2327,7 +2207,7 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="D18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2337,10 +2217,10 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" t="s">
         <v>158</v>
-      </c>
-      <c r="D19" t="s">
-        <v>159</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2349,7 +2229,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2358,7 +2238,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="D21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -2367,7 +2247,7 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="D22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2376,10 +2256,10 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" t="s">
         <v>163</v>
-      </c>
-      <c r="D23" t="s">
-        <v>164</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2388,7 +2268,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="D24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -2398,7 +2278,7 @@
       <c r="A25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E25">
         <v>0</v>

</xml_diff>

<commit_message>
lattice review up to large text changes
</commit_message>
<xml_diff>
--- a/doc/progress_tracker_2021.xlsx
+++ b/doc/progress_tracker_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaker\Documents\Thesis\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0439A534-12A9-43B0-80E4-E8FA533B25B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A8600-79EA-4480-AF3B-6DCA620FC896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="9" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="230">
   <si>
     <t>Section</t>
   </si>
@@ -650,203 +650,149 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Calendar</t>
-  </si>
-  <si>
     <t>Towards a lattice trap</t>
   </si>
   <si>
     <t>Send to S</t>
   </si>
   <si>
-    <t>June goal</t>
-  </si>
-  <si>
-    <t>June stretch goal</t>
-  </si>
-  <si>
-    <t>QD paper</t>
-  </si>
-  <si>
-    <t>Focus:</t>
-  </si>
-  <si>
-    <t>Due:</t>
-  </si>
-  <si>
-    <t>QD paper and apparatus</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>Apparatus</t>
-  </si>
-  <si>
     <t>Send to A</t>
   </si>
   <si>
-    <t>Transitions</t>
-  </si>
-  <si>
-    <t>Send to S&amp;A</t>
-  </si>
-  <si>
-    <t>QD chap</t>
-  </si>
-  <si>
-    <t>send to S&amp;A</t>
-  </si>
-  <si>
-    <t>Resubmit</t>
-  </si>
-  <si>
-    <t>QD paper -&gt; Sean</t>
-  </si>
-  <si>
-    <t>Apparatus -&gt; Andrew</t>
-  </si>
-  <si>
-    <t>lattice &amp; Main works chaps</t>
-  </si>
-  <si>
-    <t>main works chaps -&gt; S &amp; A</t>
-  </si>
-  <si>
-    <t>Lattice &amp; head/tail</t>
-  </si>
-  <si>
-    <t>Lattice chapter -&gt; Sean</t>
-  </si>
-  <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>Intro/conclusion draft</t>
-  </si>
-  <si>
-    <t>Gameplan</t>
-  </si>
-  <si>
-    <t>Proceed using master June todo</t>
-  </si>
-  <si>
-    <t>Check-off each task, count pomodoros on as estimate of time in</t>
-  </si>
-  <si>
-    <t>Reach goals</t>
-  </si>
-  <si>
     <t>Talk</t>
   </si>
   <si>
-    <t>Tuneout chapter</t>
-  </si>
-  <si>
-    <t>Adjust goals as learning along the way</t>
-  </si>
-  <si>
-    <t>If ahead of goals on June 14th, consider booking talk</t>
-  </si>
-  <si>
-    <t>Lattice &amp; Apparatus chaps, half day on talk scoping</t>
-  </si>
-  <si>
     <t>S reply</t>
   </si>
   <si>
     <t>A reply</t>
   </si>
   <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Goal due</t>
-  </si>
-  <si>
     <t>Deliver</t>
   </si>
   <si>
-    <t>Structured notes/pre-edit</t>
-  </si>
-  <si>
-    <t>July goals</t>
-  </si>
-  <si>
-    <t>Mark tasks done in calendar?</t>
-  </si>
-  <si>
-    <t>Review</t>
-  </si>
-  <si>
-    <t>Practise</t>
-  </si>
-  <si>
-    <t>Submit</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>Mostly fig changes in apparatus</t>
-  </si>
-  <si>
-    <t>Some minor text updates</t>
-  </si>
-  <si>
-    <t>MCP fig, laser cooling, TCP lock loop</t>
-  </si>
-  <si>
-    <t>DONE</t>
-  </si>
-  <si>
-    <t>Second goal:</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Th</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>SENT CH2</t>
+    <t>Chapter todo</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Wait</t>
+  </si>
+  <si>
+    <t>S revise</t>
+  </si>
+  <si>
+    <t>A revise</t>
+  </si>
+  <si>
+    <t>Total time</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total w days</t>
+  </si>
+  <si>
+    <t>Abstract/Conclusion</t>
+  </si>
+  <si>
+    <t>Test &amp; revise</t>
+  </si>
+  <si>
+    <t>Next task</t>
+  </si>
+  <si>
+    <t>Revise for A</t>
+  </si>
+  <si>
+    <t>Final review</t>
+  </si>
+  <si>
+    <t>With?</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>Draft for S</t>
+  </si>
+  <si>
+    <t>Pending A</t>
+  </si>
+  <si>
+    <t>Pending S</t>
+  </si>
+  <si>
+    <t>Done by</t>
+  </si>
+  <si>
+    <t>End August</t>
+  </si>
+  <si>
+    <t>2x revise</t>
+  </si>
+  <si>
+    <t>Further time</t>
+  </si>
+  <si>
+    <t>1 revision</t>
+  </si>
+  <si>
+    <t>Further tasks</t>
+  </si>
+  <si>
+    <t>1-2x revise</t>
+  </si>
+  <si>
+    <t>Draft for test</t>
+  </si>
+  <si>
+    <t>Revise and deliver</t>
+  </si>
+  <si>
+    <t>Inc weekend</t>
+  </si>
+  <si>
+    <t>Proof</t>
+  </si>
+  <si>
+    <t>Task list</t>
+  </si>
+  <si>
+    <t>Countdown</t>
+  </si>
+  <si>
+    <t>Dates starting</t>
+  </si>
+  <si>
+    <t>Done on time</t>
+  </si>
+  <si>
+    <t>Done faster</t>
+  </si>
+  <si>
+    <t>Done slower</t>
+  </si>
+  <si>
+    <t>Time spent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -875,8 +821,15 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -913,8 +866,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -922,91 +911,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1016,22 +925,28 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1369,7 +1284,7 @@
       </c>
       <c r="C1" s="4">
         <f ca="1">TODAY()</f>
-        <v>44357</v>
+        <v>44411</v>
       </c>
       <c r="D1" t="s">
         <v>177</v>
@@ -1384,11 +1299,11 @@
       </c>
       <c r="G2">
         <f ca="1">C1-C2</f>
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="H2">
         <f ca="1">0.8*G2</f>
-        <v>108</v>
+        <v>151.20000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1401,7 +1316,7 @@
       </c>
       <c r="D3">
         <f ca="1">C3-C1</f>
-        <v>-23</v>
+        <v>-77</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1489,7 +1404,7 @@
       </c>
       <c r="J7" s="6">
         <f t="shared" ref="J7:J14" ca="1" si="4">D7-TODAY()</f>
-        <v>-128</v>
+        <v>-182</v>
       </c>
       <c r="K7" t="s">
         <v>130</v>
@@ -1531,7 +1446,7 @@
       </c>
       <c r="J8" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>-71</v>
+        <v>-125</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1568,7 +1483,7 @@
       </c>
       <c r="J9" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>-50</v>
+        <v>-104</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1605,7 +1520,7 @@
       </c>
       <c r="J10" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>-43</v>
+        <v>-97</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1642,7 +1557,7 @@
       </c>
       <c r="J11" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>-36</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1679,7 +1594,7 @@
       </c>
       <c r="J12" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>-32</v>
+        <v>-86</v>
       </c>
       <c r="K12" t="s">
         <v>129</v>
@@ -1722,7 +1637,7 @@
       </c>
       <c r="J13" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>-30</v>
+        <v>-84</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1756,7 +1671,7 @@
       </c>
       <c r="J14" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>-23</v>
+        <v>-77</v>
       </c>
     </row>
   </sheetData>
@@ -1771,10 +1686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:R41"/>
+  <dimension ref="A2:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,10 +1697,10 @@
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" customWidth="1"/>
     <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -1810,731 +1725,972 @@
         <v>182</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="11"/>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="K5" s="10">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>179</v>
-      </c>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="K6" s="10">
-        <v>2</v>
-      </c>
-      <c r="L6" t="s">
-        <v>180</v>
-      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="22"/>
-      <c r="K7" s="24">
-        <v>3</v>
-      </c>
-      <c r="L7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8">
+      <c r="C8" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="22"/>
-      <c r="K8" s="8">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="K9" s="22"/>
-      <c r="L9" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="22"/>
-      <c r="K10" s="12"/>
-      <c r="L10" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="11"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="I13" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="15"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I14" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="J14" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="L14" s="19" t="s">
-        <v>243</v>
-      </c>
-      <c r="M14" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="O14" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="20"/>
+      <c r="C14" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" s="7">
+        <v>44403</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I15" s="9">
-        <v>31</v>
-      </c>
-      <c r="J15" s="16">
-        <v>1</v>
-      </c>
-      <c r="K15" s="16">
-        <v>2</v>
-      </c>
-      <c r="L15" s="16">
-        <v>3</v>
-      </c>
-      <c r="M15" s="16">
-        <v>4</v>
-      </c>
-      <c r="N15" s="9">
-        <v>5</v>
-      </c>
-      <c r="O15" s="16">
-        <v>6</v>
-      </c>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="17"/>
+      <c r="C15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="E17" s="26">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="18">
+        <f t="shared" ref="J17:J24" si="0">I17+G17+E17</f>
+        <v>1</v>
+      </c>
+      <c r="K17" s="11"/>
+      <c r="L17" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="11"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="K18" s="11"/>
+      <c r="L18" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" s="9">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="14">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="8">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G21" s="3">
+        <v>3</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I21" s="18">
+        <v>2</v>
+      </c>
+      <c r="J21" s="18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="G22" s="26">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I22" s="18">
+        <v>1</v>
+      </c>
+      <c r="J22" s="18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23" s="3">
+        <v>20</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G23" s="3">
+        <v>5</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I23" s="18">
+        <v>1</v>
+      </c>
+      <c r="J23" s="18">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I24" s="19">
+        <v>2</v>
+      </c>
+      <c r="J24" s="18">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E25" s="3">
+        <v>3</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I25" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="J25" s="18">
+        <f>I25+G25+E25</f>
+        <v>4.5</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G26" s="3">
+        <v>3</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="I26" s="19">
+        <v>1</v>
+      </c>
+      <c r="J26" s="18">
+        <f>I26+G26+E26</f>
+        <v>7</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I27" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="J27" s="19">
+        <f>SUM(J17:J26)</f>
+        <v>50.5</v>
+      </c>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I28" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="J28" s="19">
+        <f>J27*(7/5)</f>
+        <v>70.699999999999989</v>
+      </c>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="J29" s="17"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F31" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="21">
+        <v>44407</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="I31" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E32" t="s">
+        <v>194</v>
+      </c>
+      <c r="F32" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="21">
+        <v>44404</v>
+      </c>
+      <c r="H32" t="s">
+        <v>216</v>
+      </c>
+      <c r="I32" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="G33" s="7">
+        <v>44405</v>
+      </c>
+      <c r="H33" t="s">
+        <v>222</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E34" t="s">
+        <v>204</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
         <v>210</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="K16" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q16" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="R16" s="17"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="I34" s="11">
+        <v>2</v>
+      </c>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="E35" t="s">
+        <v>203</v>
+      </c>
+      <c r="F35" s="6">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
         <v>211</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="H35" t="s">
+        <v>214</v>
+      </c>
+      <c r="I35" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q35" s="11"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E36" t="s">
         <v>194</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q17" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="R17" s="17"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>211</v>
+      </c>
+      <c r="H36" t="s">
+        <v>218</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B37">
         <v>6</v>
       </c>
-      <c r="F18" t="s">
-        <v>182</v>
-      </c>
-      <c r="G18" t="s">
-        <v>223</v>
-      </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="17"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E19" t="s">
-        <v>195</v>
-      </c>
-      <c r="F19" t="s">
-        <v>196</v>
-      </c>
-      <c r="G19" t="s">
-        <v>225</v>
-      </c>
-      <c r="I19" s="9">
+      <c r="C37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F37">
+        <v>20</v>
+      </c>
+      <c r="G37" t="s">
+        <v>213</v>
+      </c>
+      <c r="H37" t="s">
+        <v>214</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B38">
         <v>7</v>
       </c>
-      <c r="J19" s="16">
+      <c r="C38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F38">
+        <v>0.5</v>
+      </c>
+      <c r="G38" t="s">
+        <v>211</v>
+      </c>
+      <c r="H38" t="s">
+        <v>218</v>
+      </c>
+      <c r="I38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B39">
         <v>8</v>
       </c>
-      <c r="K19" s="16">
-        <v>9</v>
-      </c>
-      <c r="L19" s="16">
-        <v>10</v>
-      </c>
-      <c r="M19" s="16">
-        <v>11</v>
-      </c>
-      <c r="N19" s="9">
-        <v>12</v>
-      </c>
-      <c r="O19" s="16">
-        <v>13</v>
-      </c>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="17"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="E20" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" t="s">
-        <v>186</v>
-      </c>
-      <c r="G20" t="s">
-        <v>222</v>
-      </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q20" s="16" t="s">
+      <c r="C39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F39">
+        <v>3</v>
+      </c>
+      <c r="G39" s="21">
+        <v>44407</v>
+      </c>
+      <c r="H39" t="s">
         <v>218</v>
       </c>
-      <c r="R20" s="17"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E21" t="s">
-        <v>197</v>
-      </c>
-      <c r="F21" t="s">
-        <v>198</v>
-      </c>
-      <c r="G21" t="s">
-        <v>221</v>
-      </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q21" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="R21" s="17"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>199</v>
-      </c>
-      <c r="F22" t="s">
-        <v>200</v>
-      </c>
-      <c r="G22" t="s">
-        <v>221</v>
-      </c>
-      <c r="I22" s="9"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="17"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
-        <v>189</v>
-      </c>
-      <c r="F23" t="s">
-        <v>201</v>
-      </c>
-      <c r="G23" t="s">
-        <v>224</v>
-      </c>
-      <c r="I23" s="9">
-        <v>14</v>
-      </c>
-      <c r="J23" s="16">
-        <v>15</v>
-      </c>
-      <c r="K23" s="16">
-        <v>16</v>
-      </c>
-      <c r="L23" s="16">
-        <v>17</v>
-      </c>
-      <c r="M23" s="16">
-        <v>18</v>
-      </c>
-      <c r="N23" s="9">
-        <v>19</v>
-      </c>
-      <c r="O23" s="16">
-        <v>20</v>
-      </c>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="17"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" t="s">
-        <v>186</v>
-      </c>
-      <c r="G24" t="s">
-        <v>223</v>
-      </c>
-      <c r="I24" s="9"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q24" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="R24" s="17"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
-        <v>234</v>
-      </c>
-      <c r="F25" t="s">
-        <v>233</v>
-      </c>
-      <c r="G25" t="s">
-        <v>223</v>
-      </c>
-      <c r="I25" s="9"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q25" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="R25" s="17"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="R26" s="17"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I27" s="9">
-        <v>21</v>
-      </c>
-      <c r="J27" s="16">
-        <v>22</v>
-      </c>
-      <c r="K27" s="16">
-        <v>23</v>
-      </c>
-      <c r="L27" s="16">
-        <v>24</v>
-      </c>
-      <c r="M27" s="16">
-        <v>25</v>
-      </c>
-      <c r="N27" s="9">
-        <v>26</v>
-      </c>
-      <c r="O27" s="16">
-        <v>27</v>
-      </c>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="17"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E28" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I28" s="9"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q28" s="16" t="s">
+      <c r="I39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D40" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="R28" s="17"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E29" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q29" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="R29" s="17"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
-        <v>214</v>
-      </c>
-      <c r="F30" t="s">
-        <v>231</v>
-      </c>
-      <c r="G30" t="s">
-        <v>225</v>
-      </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="17"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
-        <v>232</v>
-      </c>
-      <c r="G31" t="s">
-        <v>221</v>
-      </c>
-      <c r="I31" s="9">
-        <v>28</v>
-      </c>
-      <c r="J31" s="16">
-        <v>29</v>
-      </c>
-      <c r="K31" s="16">
-        <v>30</v>
-      </c>
-      <c r="L31" s="16">
-        <v>1</v>
-      </c>
-      <c r="M31" s="16">
-        <v>2</v>
-      </c>
-      <c r="N31" s="9">
+      <c r="E40" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F40">
         <v>3</v>
       </c>
-      <c r="O31" s="16">
-        <v>4</v>
-      </c>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="17"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C32" s="3"/>
-      <c r="F32" t="s">
-        <v>227</v>
-      </c>
-      <c r="G32" t="s">
-        <v>223</v>
-      </c>
-      <c r="I32" s="9"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q32" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="R32" s="17"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C33" s="3"/>
-      <c r="E33" t="s">
-        <v>215</v>
-      </c>
-      <c r="F33" t="s">
-        <v>228</v>
-      </c>
-      <c r="G33" t="s">
-        <v>223</v>
-      </c>
-      <c r="I33" s="9"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q33" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="R33" s="17"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C34" s="3"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="20"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q35" s="14"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H40" s="7"/>
+      <c r="H40" t="s">
+        <v>220</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="F41">
+        <f>SUM(F31:F40)</f>
+        <v>31.5</v>
+      </c>
+      <c r="H41" s="7"/>
+      <c r="I41">
+        <f>SUM(I31:I40)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C42" s="1"/>
+      <c r="H42" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="I42">
+        <f>I41+F41</f>
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>221</v>
+      </c>
+      <c r="I43">
+        <f>(7/5)*I42</f>
+        <v>72.099999999999994</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>133</v>
+      </c>
+      <c r="I44" s="7">
+        <f>D14+ROUNDUP(I43,0)</f>
+        <v>44476</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D13">

</xml_diff>

<commit_message>
examiner changes finished up to Gaussian beam effects
</commit_message>
<xml_diff>
--- a/doc/progress_tracker_2021.xlsx
+++ b/doc/progress_tracker_2021.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaker\Documents\Thesis\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC85A68-7F0E-47C7-BD20-83288268A266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA6680F-A004-4A9A-AFB4-31E30529593A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Minor corrections" sheetId="10" r:id="rId1"/>
-    <sheet name="Summary" sheetId="1" r:id="rId2"/>
-    <sheet name="2021" sheetId="9" r:id="rId3"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="2021" sheetId="9" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,7 +50,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>jaker:</t>
         </r>
@@ -57,7 +59,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 NB: Originally made a 20-day weekend inclusive deadline for the jan 26. Now nudgeting days spent on revision before submission</t>
@@ -72,7 +74,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>jaker:</t>
         </r>
@@ -81,7 +83,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Revision absorbed into Intro</t>
@@ -93,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="90">
   <si>
     <t>Chapter</t>
   </si>
@@ -363,256 +365,6 @@
   </si>
   <si>
     <t>Review order switched</t>
-  </si>
-  <si>
-    <t>Spectrometry --- &gt; spectrometry.</t>
-  </si>
-  <si>
-    <t>Page numbering starts on “0” instead of “1”, seems odd.</t>
-  </si>
-  <si>
-    <t>Footnote 3, “Planck” not capitalised.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> extra space after He*.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “Hydrogen”, “Helium” written with caps, should be lowercase.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> footnote – “we consider -- Doubly” --&gt; “we consider. Doubly…”.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “coefficiencts” misspelled.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> typo in GPE, should be “i \hbar” on left, rather than “-\hbar”.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “bell-type” --&gt; “Bell-type”.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “413nm” --&gt; “413 nm”.</t>
-  </si>
-  <si>
-    <t>Eq. (2.2), the subscript “lab” should not be italicised.</t>
-  </si>
-  <si>
-    <t>Missing space between number and unit in “2mm” and “1cm”.</t>
-  </si>
-  <si>
-    <t>In the footnote, “analogoous” misspelled.</t>
-  </si>
-  <si>
-    <t>Bad latex reference resulting in “??” partway down the page.</t>
-  </si>
-  <si>
-    <t>“19.8eV” missing the space before the unit.</t>
-  </si>
-  <si>
-    <t>Latex float issue(?) leading to a large space in the page.</t>
-  </si>
-  <si>
-    <t>similarly, a large space here.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “section 5.3gives” missing a space</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “smallest precision” to “highest precision”</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ref. [18], “Bose-einstein”; Ref. [19] “structure of scince”</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ref. [63], “evidence,” should be capitalised, “condesnation”</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Refs. [174, 175] duplicate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Refs. [187, 188] duplicate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Refs. [229, 230] duplicate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ref [237] “87RbD-line” missing space.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ref. [250], latex typo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ref. [351], typo “Optics COmmunications”; Ref. [353] formatting issues</t>
-  </si>
-  <si>
-    <t>line 5, “Bell-type” typo</t>
-  </si>
-  <si>
-    <t>line 4, “ molecular pumps” (extra fullstop)</t>
-  </si>
-  <si>
-    <t>line 5, fullstop missing</t>
-  </si>
-  <si>
-    <t>line 13, LVIS should be defined.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> line “…chapters ??..”</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “a.k.a.”</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “faraday” should be “Faraday”</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Is ETP the name of the manufacturer of the part?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “..1 0 ms delay ..” extra space in 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “Unforunately..”, second para, second line, typo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “dipole fibers” is too colloquial.</t>
-  </si>
-  <si>
-    <t>“…photon scattering signal…” what is it?</t>
-  </si>
-  <si>
-    <t>The RF linewidth of the crystal oscillator of 300kHz sounds excessively large.</t>
-  </si>
-  <si>
-    <t>uK in Roman font</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> \chi^2/dof ~ 1 needs a space.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “ 1140(20) MHz” should not italicized</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “also” twice..</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “…alternative approach presented in section 6.2.1”. It is section 6.2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “especially” spelt wrong.</t>
-  </si>
-  <si>
-    <t>the significance of p-value should be stated.</t>
-  </si>
-  <si>
-    <t>Page</t>
-  </si>
-  <si>
-    <t>Examiner comment</t>
-  </si>
-  <si>
-    <t>In the footnote the statement is a bit confusing as worded – it seems to imply that a collimated beam will converge to a focus.</t>
-  </si>
-  <si>
-    <t>“One of the most accessible lattice systems to realize with ultracold atoms is the Bose-Hubbard model.” – the wording is strange, just a typo(?) Bose-Hubbard is not a lattice system? Reword.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> “in Tab 5.2” inconsistent with later usage down the page, “table 5.2” and also elsewhere where “Tab. XX” is used.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> figure shows power in mW, while the caption describes the powers in Watts. Would modify the figure axis to be consistent.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Figure 6.8: From the text, it appears that these results are from the theory collaborators. They should be attributed in the figure caption.</t>
-  </si>
-  <si>
-    <t>line 10, “faraday” should be Faraday. There are several more instances of this typo in this chapter.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> First sentence: a larger range of momentum states does not necessarily mean a large phase space density.</t>
-  </si>
-  <si>
-    <t>“..transduction from photon scattering to…”, the word “transduction” means something different.</t>
-  </si>
-  <si>
-    <t>The issue of the limitation of the dynamic range should be explained. Also the contradictory issues of SNR and saturation can be dealt with two different sets of measurements, right?</t>
-  </si>
-  <si>
-    <t>“Connection to the experiment” should be emboldened (maybe just quote the section number).</t>
-  </si>
-  <si>
-    <t>“The tune-out frequency, where an atom does not interact with applied laser light…”. It is not true that at tune out frequency atoms do not interact with light, in fact, the imaginary part of the polarizability does not cancel at the tune out point.</t>
-  </si>
-  <si>
-    <t>An energy level diagram would be apt to help follow the text. “Section 5.3 gives…” needs a space.</t>
-  </si>
-  <si>
-    <t>“An equivalent model can be constructed using an LC circuit - the object of ultimate interest is the equation of motion,…” sounds very strange.</t>
-  </si>
-  <si>
-    <t>“ NIM crate..” Is NIM defined?</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>0 is even</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>No beam is perfectly collimated, and they will eventually come to a minimum waist then diverge. In any case, replaced with 'Technically speaking, the beam is not collimated in the same manner as a laser beam.
-	The divergence is reduced, but not eliminated such that the spot size remains fixed or becomes focused'</t>
-  </si>
-  <si>
-    <t>Replaced with 'One of the most accessible many-body systems to realize with ultracold bosons in an optical lattice is the Bose-Hubbard model.'</t>
-  </si>
-  <si>
-    <t>Removed acronym and left only references to the system components</t>
-  </si>
-  <si>
-    <t>Given a fixed atomic density, the statement is accurate, but I have amended to "Deeper optical dipole traps can contain more atoms at a given temperature by virtue of trapping over a larger range of particle momenta"</t>
-  </si>
-  <si>
-    <t>"The dipole beams were first aligned to overlap with the magnetic trap by piping resonant light (at 1083 nm) through the dipole beam delivery fibres instead of 1550 nm."</t>
-  </si>
-  <si>
-    <t>I think this is fine, but have changed to "The functional relationship between photon scattering and atom loss via evaporative cooling is complicated and not linear."</t>
-  </si>
-  <si>
-    <t>It's defined later in the sentence. Still, changed to "In both cases the effect of photon scattering manifests as a reduction of the total trapped final number $N$ relative to the final number $N_c$ in calibration shots."</t>
-  </si>
-  <si>
-    <t>Fair assessment. It was actually in the RF driver output. I've added a sentence "In the first case, the linewidth is a result of frequency instability in the RF drive generation system. In the second, a newer drive system was in use which afforded better performance." It might be worth fixing this as it could affect in to the in-trap cooling performance.</t>
-  </si>
-  <si>
-    <t>Changed to 'The tune-out frequency, where an atom feels no force resulting from applied laser light, is an observable that tests QED independently of the conventional measurement of energy level differences.'</t>
-  </si>
-  <si>
-    <t>Relegated LC comment to footnote</t>
-  </si>
-  <si>
-    <t>I think the XX here is a placeholder by the examiner. I have changed both instances to read 'Tab.'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latex error. The source code refs to the right section. </t>
-  </si>
-  <si>
-    <t>Not duplicated, just very similar titles. Ref 229 is an experimental result, ref 230 is theory concerning the former.</t>
-  </si>
-  <si>
-    <t>The former, amended.</t>
-  </si>
-  <si>
-    <t>This seems unnecessary, the figure is perfectly legible.</t>
   </si>
 </sst>
 </file>
@@ -639,14 +391,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -727,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -757,9 +509,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,6 +524,757 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Page</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>Done</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Examiner comment</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>Comment</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>11</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>c</v>
+          </cell>
+          <cell r="C2" t="str">
+            <v xml:space="preserve"> extra space after He*.</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>59</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>c</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>Bad latex reference resulting in “??” partway down the page.</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>59</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>c</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v xml:space="preserve"> line “…chapters ??..”</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>80</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>c</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>Latex float issue(?) leading to a large space in the page.</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>84</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>c</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>similarly, a large space here.</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>151</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>c</v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>“Connection to the experiment” should be emboldened (maybe just quote the section number).</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>192</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>c</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v xml:space="preserve"> “…alternative approach presented in section 6.2.1”. It is section 6.2.1</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v xml:space="preserve">Latex error. The source code refs to the right section. </v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>249</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>c</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v xml:space="preserve"> Ref. [250], latex typo</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>250</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>c</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v xml:space="preserve"> Ref. [351], typo “Optics COmmunications”; Ref. [353] formatting issues</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>197</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>n</v>
+          </cell>
+          <cell r="C11" t="str">
+            <v>the significance of p-value should be stated.</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>121</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C12" t="str">
+            <v>The issue of the limitation of the dynamic range should be explained. Also the contradictory issues of SNR and saturation can be dealt with two different sets of measurements, right?</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v>I have added more detail to the first paragraph of section 3.3 (formerly 4.3) explaining the upper- and lower-bounds on detectable signal, and a comment agreeing with the examiner's suggestion.</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>0</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C13" t="str">
+            <v>Page numbering starts on “0” instead of “1”, seems odd.</v>
+          </cell>
+          <cell r="D13" t="str">
+            <v>0 is even</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>173</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C14" t="str">
+            <v xml:space="preserve"> figure shows power in mW, while the caption describes the powers in Watts. Would modify the figure axis to be consistent.</v>
+          </cell>
+          <cell r="D14" t="str">
+            <v>This seems unnecessary, the figure is perfectly legible.</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>0</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C15" t="str">
+            <v>Spectrometry --- &gt; spectrometry.</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>3</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C16" t="str">
+            <v>Footnote 3, “Planck” not capitalised.</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>17</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C17" t="str">
+            <v xml:space="preserve"> “Hydrogen”, “Helium” written with caps, should be lowercase.</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>26</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C18" t="str">
+            <v xml:space="preserve"> footnote – “we consider -- Doubly” --&gt; “we consider. Doubly…”.</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>28</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C19" t="str">
+            <v xml:space="preserve"> “coefficiencts” misspelled.</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>39</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C20" t="str">
+            <v xml:space="preserve"> typo in GPE, should be “i \hbar” on left, rather than “-\hbar”.</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>44</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C21" t="str">
+            <v xml:space="preserve"> “bell-type” --&gt; “Bell-type”.</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>44</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C22" t="str">
+            <v xml:space="preserve"> “413nm” --&gt; “413 nm”.</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>44</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C23" t="str">
+            <v>line 5, “Bell-type” typo</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>45</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C24" t="str">
+            <v>line 4, “ molecular pumps” (extra fullstop)</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>45</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C25" t="str">
+            <v>line 5, fullstop missing</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>45</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C26" t="str">
+            <v>line 10, “faraday” should be Faraday. There are several more instances of this typo in this chapter.</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>45</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C27" t="str">
+            <v>line 13, LVIS should be defined.</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>50</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C28" t="str">
+            <v>In the footnote the statement is a bit confusing as worded – it seems to imply that a collimated beam will converge to a focus.</v>
+          </cell>
+          <cell r="D28" t="str">
+            <v>No beam is perfectly collimated, and they will eventually come to a minimum waist then diverge. In any case, replaced with 'Technically speaking, the beam is not collimated in the same manner as a laser beam.
+	The divergence is reduced, but not eliminated such that the spot size remains fixed or becomes focused'</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>51</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C29" t="str">
+            <v>Eq. (2.2), the subscript “lab” should not be italicised.</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>53</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C30" t="str">
+            <v>Missing space between number and unit in “2mm” and “1cm”.</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>58</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C31" t="str">
+            <v>In the footnote, “analogoous” misspelled.</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>63</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C32" t="str">
+            <v>“19.8eV” missing the space before the unit.</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>88</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C33" t="str">
+            <v>“One of the most accessible lattice systems to realize with ultracold atoms is the Bose-Hubbard model.” – the wording is strange, just a typo(?) Bose-Hubbard is not a lattice system? Reword.</v>
+          </cell>
+          <cell r="D33" t="str">
+            <v>Replaced with 'One of the most accessible many-body systems to realize with ultracold bosons in an optical lattice is the Bose-Hubbard model.'</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>91</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C34" t="str">
+            <v xml:space="preserve"> “a.k.a.”</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>95</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C35" t="str">
+            <v xml:space="preserve"> “faraday” should be “Faraday”</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>95</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C36" t="str">
+            <v xml:space="preserve"> Is ETP the name of the manufacturer of the part?</v>
+          </cell>
+          <cell r="D36" t="str">
+            <v>The former, amended.</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>103</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C37" t="str">
+            <v xml:space="preserve"> “..1 0 ms delay ..” extra space in 10</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>104</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C38" t="str">
+            <v xml:space="preserve"> “Unforunately..”, second para, second line, typo</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>104</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C39" t="str">
+            <v>“ NIM crate..” Is NIM defined?</v>
+          </cell>
+          <cell r="D39" t="str">
+            <v>Removed acronym and left only references to the system components</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>106</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C40" t="str">
+            <v xml:space="preserve"> First sentence: a larger range of momentum states does not necessarily mean a large phase space density.</v>
+          </cell>
+          <cell r="D40" t="str">
+            <v>Given a fixed atomic density, the statement is accurate, but I have amended to "Deeper optical dipole traps can contain more atoms at a given temperature by virtue of trapping over a larger range of particle momenta"</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>107</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C41" t="str">
+            <v xml:space="preserve"> “dipole fibers” is too colloquial.</v>
+          </cell>
+          <cell r="D41" t="str">
+            <v>"The dipole beams were first aligned to overlap with the magnetic trap by piping resonant light (at 1083 nm) through the dipole beam delivery fibres instead of 1550 nm."</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>119</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C42" t="str">
+            <v>“…photon scattering signal…” what is it?</v>
+          </cell>
+          <cell r="D42" t="str">
+            <v>It's defined later in the sentence. Still, changed to "In both cases the effect of photon scattering manifests as a reduction of the total trapped final number $N$ relative to the final number $N_c$ in calibration shots."</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>121</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C43" t="str">
+            <v>“..transduction from photon scattering to…”, the word “transduction” means something different.</v>
+          </cell>
+          <cell r="D43" t="str">
+            <v>I think this is fine, but have changed to "The functional relationship between photon scattering and atom loss via evaporative cooling is complicated and not linear."</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>126</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C44" t="str">
+            <v>uK in Roman font</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>130</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C45" t="str">
+            <v>The RF linewidth of the crystal oscillator of 300kHz sounds excessively large.</v>
+          </cell>
+          <cell r="D45" t="str">
+            <v>Fair assessment. It was actually in the RF driver output. I've added a sentence "In the first case, the linewidth is a result of frequency instability in the RF drive generation system. In the second, a newer drive system was in use which afforded better performance." It might be worth fixing this as it could affect in to the in-trap cooling performance.</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>134</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C46" t="str">
+            <v xml:space="preserve"> “section 5.3gives” missing a space</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>135</v>
+          </cell>
+          <cell r="B47" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C47" t="str">
+            <v>“The tune-out frequency, where an atom does not interact with applied laser light…”. It is not true that at tune out frequency atoms do not interact with light, in fact, the imaginary part of the polarizability does not cancel at the tune out point.</v>
+          </cell>
+          <cell r="D47" t="str">
+            <v>Changed to 'The tune-out frequency, where an atom feels no force resulting from applied laser light, is an observable that tests QED independently of the conventional measurement of energy level differences.'</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>136</v>
+          </cell>
+          <cell r="B48" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C48" t="str">
+            <v>“An equivalent model can be constructed using an LC circuit - the object of ultimate interest is the equation of motion,…” sounds very strange.</v>
+          </cell>
+          <cell r="D48" t="str">
+            <v>Relegated LC comment to footnote</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>167</v>
+          </cell>
+          <cell r="B49" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C49" t="str">
+            <v xml:space="preserve"> \chi^2/dof ~ 1 needs a space.</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>169</v>
+          </cell>
+          <cell r="B50" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C50" t="str">
+            <v xml:space="preserve"> “in Tab 5.2” inconsistent with later usage down the page, “table 5.2” and also elsewhere where “Tab. XX” is used.</v>
+          </cell>
+          <cell r="D50" t="str">
+            <v>I think the XX here is a placeholder by the examiner. I have changed both instances to read 'Tab.'</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>169</v>
+          </cell>
+          <cell r="B51" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C51" t="str">
+            <v xml:space="preserve"> “ 1140(20) MHz” should not italicized</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>171</v>
+          </cell>
+          <cell r="B52" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C52" t="str">
+            <v xml:space="preserve"> “also” twice..</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53">
+            <v>181</v>
+          </cell>
+          <cell r="B53" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C53" t="str">
+            <v xml:space="preserve"> “smallest precision” to “highest precision”</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54">
+            <v>194</v>
+          </cell>
+          <cell r="B54" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C54" t="str">
+            <v xml:space="preserve"> “especially” spelt wrong.</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55">
+            <v>208</v>
+          </cell>
+          <cell r="B55" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C55" t="str">
+            <v xml:space="preserve"> Figure 6.8: From the text, it appears that these results are from the theory collaborators. They should be attributed in the figure caption.</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56">
+            <v>224</v>
+          </cell>
+          <cell r="B56" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C56" t="str">
+            <v xml:space="preserve"> Ref. [18], “Bose-einstein”; Ref. [19] “structure of scince”</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57">
+            <v>227</v>
+          </cell>
+          <cell r="B57" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C57" t="str">
+            <v xml:space="preserve"> Ref. [63], “evidence,” should be capitalised, “condesnation”</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58">
+            <v>236</v>
+          </cell>
+          <cell r="B58" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C58" t="str">
+            <v xml:space="preserve"> Refs. [174, 175] duplicate.</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59">
+            <v>237</v>
+          </cell>
+          <cell r="B59" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C59" t="str">
+            <v xml:space="preserve"> Refs. [187, 188] duplicate.</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>240</v>
+          </cell>
+          <cell r="B60" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C60" t="str">
+            <v xml:space="preserve"> Refs. [229, 230] duplicate.</v>
+          </cell>
+          <cell r="D60" t="str">
+            <v>Not duplicated, just very similar titles. Ref 229 is an experimental result, ref 230 is theory concerning the former.</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61">
+            <v>241</v>
+          </cell>
+          <cell r="B61" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C61" t="str">
+            <v xml:space="preserve"> Ref [237] “87RbD-line” missing space.</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62">
+            <v>134</v>
+          </cell>
+          <cell r="B62" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="C62" t="str">
+            <v>An energy level diagram would be apt to help follow the text. “Section 5.3 gives…” needs a space.</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1073,778 +1573,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A0C1BF-E025-4B76-B3E9-58E25C8C700F}">
-  <dimension ref="A1:D62"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="103.28515625" customWidth="1"/>
-    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>59</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>59</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>80</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>84</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>151</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>192</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>249</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>250</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>121</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>173</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C13" t="s">
-        <v>142</v>
-      </c>
-      <c r="D13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>197</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>28</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>44</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>44</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>44</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C23" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>45</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>45</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>45</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>45</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C27" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>50</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>51</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>53</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C30" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>58</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C31" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>63</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>88</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C33" t="s">
-        <v>140</v>
-      </c>
-      <c r="D33" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>91</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C34" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>95</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>95</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C36" t="s">
-        <v>124</v>
-      </c>
-      <c r="D36" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>103</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C37" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>104</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C38" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>104</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C39" t="s">
-        <v>152</v>
-      </c>
-      <c r="D39" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>106</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C40" t="s">
-        <v>145</v>
-      </c>
-      <c r="D40" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>107</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" t="s">
-        <v>127</v>
-      </c>
-      <c r="D41" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>119</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C42" t="s">
-        <v>128</v>
-      </c>
-      <c r="D42" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>121</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C43" t="s">
-        <v>146</v>
-      </c>
-      <c r="D43" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>126</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C44" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>130</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C45" t="s">
-        <v>129</v>
-      </c>
-      <c r="D45" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>134</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C46" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>135</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C47" t="s">
-        <v>149</v>
-      </c>
-      <c r="D47" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>136</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C48" t="s">
-        <v>151</v>
-      </c>
-      <c r="D48" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>167</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C49" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>169</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C50" t="s">
-        <v>141</v>
-      </c>
-      <c r="D50" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>169</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C51" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>171</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C52" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>181</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C53" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>194</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C54" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>208</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C55" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>224</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C56" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>227</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C57" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>236</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C58" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>237</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C59" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>240</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C60" t="s">
-        <v>113</v>
-      </c>
-      <c r="D60" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>241</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C61" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>134</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C62" t="s">
-        <v>150</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D62">
-    <sortCondition ref="B2:B62"/>
-  </sortState>
-  <conditionalFormatting sqref="B2:B62">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:V80"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -3009,7 +2741,7 @@
       </c>
       <c r="D29" s="3">
         <f ca="1">TODAY()</f>
-        <v>44667</v>
+        <v>44731</v>
       </c>
       <c r="H29" t="s">
         <v>73</v>
@@ -3304,7 +3036,7 @@
       </c>
       <c r="I44" s="6">
         <f ca="1">D29+ROUNDUP(I43,0)</f>
-        <v>44673</v>
+        <v>44737</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -3462,7 +3194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C086C7-B733-4A1C-8B30-B043A00420F4}">
   <dimension ref="A1:L14"/>
   <sheetViews>
@@ -3487,7 +3219,7 @@
       </c>
       <c r="C1" s="3">
         <f ca="1">TODAY()</f>
-        <v>44667</v>
+        <v>44731</v>
       </c>
       <c r="D1" t="s">
         <v>36</v>
@@ -3502,11 +3234,11 @@
       </c>
       <c r="G2">
         <f ca="1">C1-C2</f>
-        <v>445</v>
+        <v>509</v>
       </c>
       <c r="H2">
         <f ca="1">0.8*G2</f>
-        <v>356</v>
+        <v>407.20000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3519,7 +3251,7 @@
       </c>
       <c r="D3">
         <f ca="1">C3-C1</f>
-        <v>-333</v>
+        <v>-397</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3607,7 +3339,7 @@
       </c>
       <c r="J7" s="5">
         <f t="shared" ref="J7:J14" ca="1" si="4">D7-TODAY()</f>
-        <v>-438</v>
+        <v>-502</v>
       </c>
       <c r="K7" t="s">
         <v>22</v>
@@ -3649,7 +3381,7 @@
       </c>
       <c r="J8" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-381</v>
+        <v>-445</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3686,7 +3418,7 @@
       </c>
       <c r="J9" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-360</v>
+        <v>-424</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3723,7 +3455,7 @@
       </c>
       <c r="J10" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-353</v>
+        <v>-417</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3760,7 +3492,7 @@
       </c>
       <c r="J11" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-346</v>
+        <v>-410</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3797,7 +3529,7 @@
       </c>
       <c r="J12" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-342</v>
+        <v>-406</v>
       </c>
       <c r="K12" t="s">
         <v>21</v>
@@ -3840,7 +3572,7 @@
       </c>
       <c r="J13" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-340</v>
+        <v>-404</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3874,7 +3606,7 @@
       </c>
       <c r="J14" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>-333</v>
+        <v>-397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>